<commit_message>
update spesifikasi struktur baja
</commit_message>
<xml_diff>
--- a/data-ikan.xlsx
+++ b/data-ikan.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/macbook/ruang-kerja/input-excel/selenium-data-excel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ruang-kerja\e-katalog\input-excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAEED94A-BFE6-A04F-8342-722EA7B0D445}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41D4B70D-BB82-4A1A-AEEB-6B6F6C4E2FD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="20740" windowHeight="11760" xr2:uid="{332B21BA-2D9F-4858-874B-A51052F96E41}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="1" xr2:uid="{332B21BA-2D9F-4858-874B-A51052F96E41}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="48">
   <si>
     <t>Pompa Air Alkon dan Kelengkapan</t>
   </si>
@@ -145,6 +145,42 @@
   </si>
   <si>
     <t>31-12-2023</t>
+  </si>
+  <si>
+    <t>12-12-2023</t>
+  </si>
+  <si>
+    <t>Masa Pemeliharaan</t>
+  </si>
+  <si>
+    <t>Gambar Teknis</t>
+  </si>
+  <si>
+    <t>Spesifikasi Teknis</t>
+  </si>
+  <si>
+    <t>Nomor Surat Perjanjian Penyediaan Material</t>
+  </si>
+  <si>
+    <t>Masa Berlaku Surat Perjanjian Penyediaan Material</t>
+  </si>
+  <si>
+    <t>Peralatan Kerja Utama</t>
+  </si>
+  <si>
+    <t>Personil Manajerial</t>
+  </si>
+  <si>
+    <t>Pengalaman Kerja Perusahaan</t>
+  </si>
+  <si>
+    <t>Dokumen Rencana Keselamatan Konstruksi (RKK)</t>
+  </si>
+  <si>
+    <t>Sisa Kemampuan Paket (SKP)</t>
+  </si>
+  <si>
+    <t>Komponen Biaya</t>
   </si>
 </sst>
 </file>
@@ -283,8 +319,8 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
@@ -605,23 +641,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4CB6367-EB8F-4C1C-887F-7E56E11A17F3}">
   <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:G5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="56.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="56.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="56.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="56.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>19</v>
       </c>
@@ -650,7 +686,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -664,7 +700,7 @@
         <v>31</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F2">
         <v>1000</v>
@@ -679,7 +715,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -708,7 +744,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -737,7 +773,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -766,14 +802,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B6" s="3"/>
       <c r="C6" s="2"/>
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
       <c r="F6" s="4"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="6"/>
       <c r="B7" s="3"/>
       <c r="C7" s="2"/>
@@ -781,7 +817,7 @@
       <c r="E7" s="5"/>
       <c r="F7" s="4"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="6"/>
       <c r="B8" s="3"/>
       <c r="C8" s="2"/>
@@ -789,14 +825,14 @@
       <c r="E8" s="5"/>
       <c r="F8" s="4"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B9" s="3"/>
       <c r="C9" s="2"/>
       <c r="D9" s="5"/>
       <c r="E9" s="5"/>
       <c r="F9" s="4"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="6"/>
       <c r="B10" s="3"/>
       <c r="C10" s="2"/>
@@ -804,7 +840,7 @@
       <c r="E10" s="5"/>
       <c r="F10" s="4"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="6"/>
       <c r="B11" s="3"/>
       <c r="C11" s="2"/>
@@ -812,7 +848,7 @@
       <c r="E11" s="5"/>
       <c r="F11" s="4"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="6"/>
       <c r="B12" s="3"/>
       <c r="C12" s="2"/>
@@ -820,7 +856,7 @@
       <c r="E12" s="5"/>
       <c r="F12" s="4"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="6"/>
       <c r="B13" s="3"/>
       <c r="C13" s="2"/>
@@ -828,7 +864,7 @@
       <c r="E13" s="5"/>
       <c r="F13" s="4"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="6"/>
       <c r="B14" s="3"/>
       <c r="C14" s="2"/>
@@ -836,7 +872,7 @@
       <c r="E14" s="5"/>
       <c r="F14" s="4"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="6"/>
       <c r="B15" s="3"/>
       <c r="C15" s="2"/>
@@ -844,7 +880,7 @@
       <c r="E15" s="5"/>
       <c r="F15" s="4"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="6"/>
       <c r="B16" s="3"/>
       <c r="C16" s="2"/>
@@ -852,7 +888,7 @@
       <c r="E16" s="5"/>
       <c r="F16" s="4"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="6"/>
       <c r="B17" s="3"/>
       <c r="C17" s="2"/>
@@ -860,7 +896,7 @@
       <c r="E17" s="5"/>
       <c r="F17" s="4"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="6"/>
       <c r="B18" s="3"/>
       <c r="C18" s="2"/>
@@ -868,7 +904,7 @@
       <c r="E18" s="5"/>
       <c r="F18" s="4"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="6"/>
       <c r="B19" s="3"/>
       <c r="C19" s="2"/>
@@ -876,7 +912,7 @@
       <c r="E19" s="5"/>
       <c r="F19" s="4"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="6"/>
       <c r="B20" s="3"/>
       <c r="C20" s="2"/>
@@ -892,28 +928,22 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97859F92-A8B8-4CB4-9D01-C745FB9E23C0}">
-  <dimension ref="A2:J2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C4DDC65-33C5-4D8A-8177-3A4BF7C22B88}">
+  <sheetPr codeName="Lembar2"/>
+  <dimension ref="A2:U2"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="U2" sqref="U2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="17.83203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="41.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="47.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="20.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>7</v>
       </c>
@@ -943,6 +973,39 @@
       </c>
       <c r="J2" t="s">
         <v>18</v>
+      </c>
+      <c r="K2" t="s">
+        <v>37</v>
+      </c>
+      <c r="L2" t="s">
+        <v>38</v>
+      </c>
+      <c r="M2" t="s">
+        <v>39</v>
+      </c>
+      <c r="N2" t="s">
+        <v>40</v>
+      </c>
+      <c r="O2" t="s">
+        <v>41</v>
+      </c>
+      <c r="P2" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>43</v>
+      </c>
+      <c r="R2" t="s">
+        <v>44</v>
+      </c>
+      <c r="S2" t="s">
+        <v>45</v>
+      </c>
+      <c r="T2" t="s">
+        <v>46</v>
+      </c>
+      <c r="U2" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>